<commit_message>
Renamed from piLang to pyLang
</commit_message>
<xml_diff>
--- a/test/go_card_profile.xlsx
+++ b/test/go_card_profile.xlsx
@@ -634,7 +634,7 @@
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>Ormiston station</t>
+          <t>Redbank station</t>
         </is>
       </c>
       <c r="S4" t="n">
@@ -699,7 +699,7 @@
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>Airport Drive, Airport (Brisbane), Brisbane East</t>
+          <t>Grey Street, South Brisbane, Brisbane Central</t>
         </is>
       </c>
       <c r="S5" t="n">

</xml_diff>